<commit_message>
valuation of champaa final, struc of padam final, bindabasini mandir dhalan baato estimate 15.7m, kalimasta mandir valuation final
</commit_message>
<xml_diff>
--- a/ofc/estimates/bindabasini mandir jane sadak dhalaan/estimate.xlsx
+++ b/ofc/estimates/bindabasini mandir jane sadak dhalaan/estimate.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\081-082\ofc\estimates\bindabasini mandir jane sadak dhalaan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\081_082\ofc\ofc\estimates\bindabasini mandir jane sadak dhalaan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="WCR" sheetId="6" r:id="rId1"/>
@@ -42,7 +42,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'bendol estimate'!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">WCR!$1:$12</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -236,11 +236,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -399,7 +399,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -409,7 +409,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -430,14 +430,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -446,7 +446,7 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -471,7 +471,7 @@
     <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -504,7 +504,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -513,7 +513,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -528,7 +528,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -544,17 +544,35 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -579,22 +597,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -606,18 +618,6 @@
     </xf>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1241,106 +1241,106 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="79" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-    </row>
-    <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="80" t="s">
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+    </row>
+    <row r="2" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A2" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="81" t="s">
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="81"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-    </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="81" t="s">
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="81"/>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="81"/>
-    </row>
-    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="82" t="s">
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+    </row>
+    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="82"/>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="82"/>
-      <c r="H5" s="82"/>
-      <c r="I5" s="82"/>
-      <c r="J5" s="82"/>
-      <c r="K5" s="82"/>
-    </row>
-    <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="74"/>
+    </row>
+    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="9"/>
-      <c r="C6" s="77" t="e">
+      <c r="C6" s="69" t="e">
         <f>F18</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="78"/>
+      <c r="D6" s="70"/>
       <c r="E6" s="10"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
@@ -1348,90 +1348,90 @@
         <v>20</v>
       </c>
       <c r="I6" s="9"/>
-      <c r="J6" s="77" t="e">
+      <c r="J6" s="69" t="e">
         <f>I18</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="78"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K6" s="70"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="I7" s="73" t="s">
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
+      <c r="I7" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="73"/>
-      <c r="K7" s="73"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="71" t="e">
+      <c r="J7" s="79"/>
+      <c r="K7" s="79"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="77" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="I8" s="74" t="s">
+      <c r="B8" s="77"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="77"/>
+      <c r="I8" s="80" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="74"/>
-      <c r="K8" s="74"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="75" t="e">
+      <c r="J8" s="80"/>
+      <c r="K8" s="80"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="81" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B9" s="75"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="I9" s="74" t="s">
+      <c r="B9" s="81"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="81"/>
+      <c r="F9" s="81"/>
+      <c r="I9" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="74"/>
-      <c r="K9" s="74"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="69" t="s">
+      <c r="J9" s="80"/>
+      <c r="K9" s="80"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="69" t="s">
+      <c r="B11" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="69" t="s">
+      <c r="C11" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="76" t="s">
+      <c r="D11" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="76" t="s">
+      <c r="E11" s="82"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="76"/>
-      <c r="I11" s="76"/>
-      <c r="J11" s="69" t="s">
+      <c r="H11" s="82"/>
+      <c r="I11" s="82"/>
+      <c r="J11" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="70" t="s">
+      <c r="K11" s="76" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="69"/>
-      <c r="B12" s="69"/>
-      <c r="C12" s="69"/>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="75"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="75"/>
       <c r="D12" s="12" t="s">
         <v>26</v>
       </c>
@@ -1450,10 +1450,10 @@
       <c r="I12" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="69"/>
-      <c r="K12" s="70"/>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J12" s="75"/>
+      <c r="K12" s="76"/>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="28" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -1496,7 +1496,7 @@
       </c>
       <c r="K13" s="15"/>
     </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="28"/>
       <c r="B14" s="34" t="e">
         <f>#REF!</f>
@@ -1518,7 +1518,7 @@
       <c r="J14" s="29"/>
       <c r="K14" s="15"/>
     </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="30"/>
       <c r="B15" s="30"/>
       <c r="C15" s="13"/>
@@ -1531,7 +1531,7 @@
       <c r="J15" s="29"/>
       <c r="K15" s="15"/>
     </row>
-    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="28" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -1574,7 +1574,7 @@
       </c>
       <c r="K16" s="15"/>
     </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="30"/>
       <c r="B17" s="30"/>
       <c r="C17" s="13"/>
@@ -1587,7 +1587,7 @@
       <c r="J17" s="29"/>
       <c r="K17" s="15"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="6" t="s">
         <v>16</v>
@@ -1613,13 +1613,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -1633,6 +1626,13 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1650,134 +1650,134 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:F7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="5.88671875" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="88" t="s">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="88"/>
-      <c r="K1" s="88"/>
-    </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="89" t="s">
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-    </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="81" t="s">
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+    </row>
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="81"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-    </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="81" t="s">
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+    </row>
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="81"/>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="81"/>
-    </row>
-    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="90" t="s">
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+    </row>
+    <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="90"/>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
-      <c r="H5" s="90"/>
-      <c r="I5" s="90"/>
-      <c r="J5" s="90"/>
-      <c r="K5" s="90"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="71" t="s">
+      <c r="B5" s="86"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="86"/>
+      <c r="K5" s="86"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="71"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
+      <c r="B6" s="77"/>
+      <c r="C6" s="77"/>
+      <c r="D6" s="77"/>
+      <c r="E6" s="77"/>
+      <c r="F6" s="77"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="87" t="s">
+      <c r="H6" s="83" t="s">
         <v>49</v>
       </c>
-      <c r="I6" s="87"/>
-      <c r="J6" s="87"/>
-      <c r="K6" s="87"/>
-    </row>
-    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="84" t="s">
+      <c r="I6" s="83"/>
+      <c r="J6" s="83"/>
+      <c r="K6" s="83"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="84"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
+      <c r="B7" s="88"/>
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="85" t="s">
+      <c r="H7" s="89" t="s">
         <v>55</v>
       </c>
-      <c r="I7" s="85"/>
-      <c r="J7" s="85"/>
-      <c r="K7" s="85"/>
-    </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="89"/>
+      <c r="J7" s="89"/>
+      <c r="K7" s="89"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="150" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A9" s="30">
         <v>1</v>
       </c>
@@ -1838,7 +1838,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19"/>
       <c r="B10" s="39" t="s">
         <v>43</v>
@@ -1847,7 +1847,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="40">
-        <v>15</v>
+        <v>15.7</v>
       </c>
       <c r="E10" s="40">
         <f>14/3.281</f>
@@ -1858,7 +1858,7 @@
       </c>
       <c r="G10" s="41">
         <f>PRODUCT(C10:F10)</f>
-        <v>9.600731484303564</v>
+        <v>10.048765620237731</v>
       </c>
       <c r="H10" s="42"/>
       <c r="I10" s="42"/>
@@ -1872,7 +1872,7 @@
       <c r="R10" s="26"/>
       <c r="S10" s="26"/>
     </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19"/>
       <c r="B11" s="39" t="s">
         <v>42</v>
@@ -1883,7 +1883,7 @@
       <c r="F11" s="22"/>
       <c r="G11" s="24">
         <f>SUM(G10:G10)</f>
-        <v>9.600731484303564</v>
+        <v>10.048765620237731</v>
       </c>
       <c r="H11" s="23" t="s">
         <v>41</v>
@@ -1893,7 +1893,7 @@
       </c>
       <c r="J11" s="43">
         <f>G11*I11</f>
-        <v>620.4952758305393</v>
+        <v>649.45172203596451</v>
       </c>
       <c r="K11" s="22"/>
       <c r="M11" s="26"/>
@@ -1904,7 +1904,7 @@
       <c r="R11" s="26"/>
       <c r="S11" s="26"/>
     </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19"/>
       <c r="B12" s="39" t="s">
         <v>40</v>
@@ -1918,7 +1918,7 @@
       <c r="I12" s="24"/>
       <c r="J12" s="43">
         <f>0.13*G11*19284/360</f>
-        <v>66.856293812861921</v>
+        <v>69.976254190795487</v>
       </c>
       <c r="K12" s="22"/>
       <c r="M12" s="26"/>
@@ -1929,7 +1929,7 @@
       <c r="R12" s="26"/>
       <c r="S12" s="26"/>
     </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19"/>
       <c r="B13" s="39"/>
       <c r="C13" s="20"/>
@@ -1949,7 +1949,7 @@
       <c r="R13" s="26"/>
       <c r="S13" s="26"/>
     </row>
-    <row r="14" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
         <v>2</v>
       </c>
@@ -1973,7 +1973,7 @@
       <c r="R14" s="26"/>
       <c r="S14" s="26"/>
     </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19"/>
       <c r="B15" s="39" t="str">
         <f>B10</f>
@@ -1985,7 +1985,7 @@
       </c>
       <c r="D15" s="40">
         <f>D10</f>
-        <v>15</v>
+        <v>15.7</v>
       </c>
       <c r="E15" s="40">
         <f>E10</f>
@@ -1996,7 +1996,7 @@
       </c>
       <c r="G15" s="41">
         <f>PRODUCT(C15:F15)</f>
-        <v>9.600731484303564</v>
+        <v>10.048765620237731</v>
       </c>
       <c r="H15" s="42"/>
       <c r="I15" s="42"/>
@@ -2010,7 +2010,7 @@
       <c r="R15" s="26"/>
       <c r="S15" s="26"/>
     </row>
-    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="42"/>
       <c r="B16" s="39" t="s">
         <v>42</v>
@@ -2021,7 +2021,7 @@
       <c r="F16" s="45"/>
       <c r="G16" s="35">
         <f>SUM(G15:G15)</f>
-        <v>9.600731484303564</v>
+        <v>10.048765620237731</v>
       </c>
       <c r="H16" s="35" t="s">
         <v>41</v>
@@ -2031,11 +2031,11 @@
       </c>
       <c r="J16" s="46">
         <f>G16*I16</f>
-        <v>43794.024687595236</v>
+        <v>45837.745839683012</v>
       </c>
       <c r="K16" s="38"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="42"/>
       <c r="B17" s="39" t="s">
         <v>40</v>
@@ -2049,11 +2049,11 @@
       <c r="I17" s="45"/>
       <c r="J17" s="47">
         <f>0.13*G16*(15452.6/5)</f>
-        <v>3857.262846693081</v>
+        <v>4037.2684462054249</v>
       </c>
       <c r="K17" s="38"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="42"/>
       <c r="B18" s="39"/>
       <c r="C18" s="44"/>
@@ -2066,7 +2066,7 @@
       <c r="J18" s="47"/>
       <c r="K18" s="38"/>
     </row>
-    <row r="19" spans="1:19" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" s="1" customFormat="1" ht="69" x14ac:dyDescent="0.3">
       <c r="A19" s="65">
         <v>3</v>
       </c>
@@ -2091,7 +2091,7 @@
       <c r="J19" s="47"/>
       <c r="K19" s="30"/>
     </row>
-    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="42"/>
       <c r="B20" s="39" t="str">
         <f>B15</f>
@@ -2099,30 +2099,30 @@
       </c>
       <c r="C20" s="44">
         <f>TRUNC(D21/0.15,0)</f>
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D20" s="45">
         <f>E15-0.1</f>
         <v>4.1669917708015847</v>
       </c>
       <c r="E20" s="45">
-        <f>10*10/162</f>
-        <v>0.61728395061728392</v>
+        <f>8*8/162</f>
+        <v>0.39506172839506171</v>
       </c>
       <c r="F20" s="45">
         <f>PRODUCT(C20:E20)</f>
-        <v>252.07727996207115</v>
+        <v>167.91433506044902</v>
       </c>
       <c r="G20" s="45">
         <f>F20/1000</f>
-        <v>0.25207727996207113</v>
+        <v>0.16791433506044903</v>
       </c>
       <c r="H20" s="45"/>
       <c r="I20" s="45"/>
       <c r="J20" s="47"/>
       <c r="K20" s="38"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="44">
@@ -2131,7 +2131,7 @@
       </c>
       <c r="D21" s="7">
         <f>D15-0.1*3</f>
-        <v>14.7</v>
+        <v>15.399999999999999</v>
       </c>
       <c r="E21" s="45">
         <f>8*8/162</f>
@@ -2139,11 +2139,11 @@
       </c>
       <c r="F21" s="45">
         <f>PRODUCT(C21:E21)</f>
-        <v>156.79999999999998</v>
+        <v>164.26666666666665</v>
       </c>
       <c r="G21" s="45">
         <f>F21/1000</f>
-        <v>0.15679999999999999</v>
+        <v>0.16426666666666664</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -2152,7 +2152,7 @@
       <c r="M21" s="68"/>
       <c r="N21" s="68"/>
     </row>
-    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="42"/>
       <c r="B22" s="39" t="s">
         <v>42</v>
@@ -2163,7 +2163,7 @@
       <c r="F22" s="45"/>
       <c r="G22" s="35">
         <f>SUM(G20:G21)</f>
-        <v>0.40887727996207113</v>
+        <v>0.33218100172711568</v>
       </c>
       <c r="H22" s="35" t="s">
         <v>41</v>
@@ -2173,11 +2173,11 @@
       </c>
       <c r="J22" s="46">
         <f>G22*I22</f>
-        <v>50758.025534491513</v>
+        <v>41236.949554404142</v>
       </c>
       <c r="K22" s="38"/>
     </row>
-    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="42"/>
       <c r="B23" s="39" t="s">
         <v>40</v>
@@ -2191,11 +2191,11 @@
       <c r="I23" s="45"/>
       <c r="J23" s="47">
         <f>0.13*G22*110960</f>
-        <v>5897.9729879968845</v>
+        <v>4791.6445137132987</v>
       </c>
       <c r="K23" s="38"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -2208,7 +2208,7 @@
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
     </row>
-    <row r="25" spans="1:19" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" s="1" customFormat="1" ht="69" x14ac:dyDescent="0.3">
       <c r="A25" s="65">
         <v>4</v>
       </c>
@@ -2225,7 +2225,7 @@
       <c r="J25" s="47"/>
       <c r="K25" s="30"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="42"/>
       <c r="B26" s="25" t="str">
         <f>B15</f>
@@ -2237,7 +2237,7 @@
       </c>
       <c r="D26" s="45">
         <f>D15</f>
-        <v>15</v>
+        <v>15.7</v>
       </c>
       <c r="E26" s="45">
         <f>E15</f>
@@ -2248,14 +2248,14 @@
       </c>
       <c r="G26" s="41">
         <f>PRODUCT(C26:F26)</f>
-        <v>9.600731484303564</v>
+        <v>10.048765620237731</v>
       </c>
       <c r="H26" s="45"/>
       <c r="I26" s="45"/>
       <c r="J26" s="47"/>
       <c r="K26" s="38"/>
     </row>
-    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="42"/>
       <c r="B27" s="39" t="s">
         <v>42</v>
@@ -2266,7 +2266,7 @@
       <c r="F27" s="45"/>
       <c r="G27" s="35">
         <f>SUM(G26:G26)</f>
-        <v>9.600731484303564</v>
+        <v>10.048765620237731</v>
       </c>
       <c r="H27" s="35" t="s">
         <v>41</v>
@@ -2276,11 +2276,11 @@
       </c>
       <c r="J27" s="46">
         <f>G27*I27</f>
-        <v>111254.90856446204</v>
+        <v>116446.80429747027</v>
       </c>
       <c r="K27" s="38"/>
     </row>
-    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="42"/>
       <c r="B28" s="39" t="s">
         <v>40</v>
@@ -2294,11 +2294,11 @@
       <c r="I28" s="45"/>
       <c r="J28" s="47">
         <f>0.13*G27*((128662.2+6685.5)/15)</f>
-        <v>11261.786680889971</v>
+        <v>11787.336725998171</v>
       </c>
       <c r="K28" s="38"/>
     </row>
-    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="42"/>
       <c r="B29" s="39"/>
       <c r="C29" s="44"/>
@@ -2311,7 +2311,7 @@
       <c r="J29" s="47"/>
       <c r="K29" s="38"/>
     </row>
-    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="19">
         <v>5</v>
       </c>
@@ -2347,7 +2347,7 @@
       <c r="R30" s="26"/>
       <c r="S30" s="26"/>
     </row>
-    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="19"/>
       <c r="B31" s="25"/>
       <c r="C31" s="20"/>
@@ -2367,7 +2367,7 @@
       <c r="R31" s="26"/>
       <c r="S31" s="26"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="42"/>
       <c r="B32" s="48" t="s">
         <v>17</v>
@@ -2381,11 +2381,11 @@
       <c r="I32" s="43"/>
       <c r="J32" s="43">
         <f>SUM(J10:J30)</f>
-        <v>228011.33287177212</v>
+        <v>225357.17735370109</v>
       </c>
       <c r="K32" s="38"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="60"/>
       <c r="B33" s="63"/>
       <c r="C33" s="64"/>
@@ -2398,16 +2398,16 @@
       <c r="J33" s="62"/>
       <c r="K33" s="59"/>
     </row>
-    <row r="34" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="52"/>
       <c r="B34" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="83">
+      <c r="C34" s="87">
         <f>J32</f>
-        <v>228011.33287177212</v>
-      </c>
-      <c r="D34" s="83"/>
+        <v>225357.17735370109</v>
+      </c>
+      <c r="D34" s="87"/>
       <c r="E34" s="41">
         <v>100</v>
       </c>
@@ -2418,15 +2418,15 @@
       <c r="J34" s="56"/>
       <c r="K34" s="57"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="58"/>
       <c r="B35" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="86">
+      <c r="C35" s="90">
         <v>200000</v>
       </c>
-      <c r="D35" s="86"/>
+      <c r="D35" s="90"/>
       <c r="E35" s="41"/>
       <c r="F35" s="51"/>
       <c r="G35" s="50"/>
@@ -2435,19 +2435,19 @@
       <c r="J35" s="50"/>
       <c r="K35" s="51"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="58"/>
       <c r="B36" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="86">
+      <c r="C36" s="90">
         <f>C35-C38-C39</f>
         <v>190000</v>
       </c>
-      <c r="D36" s="86"/>
+      <c r="D36" s="90"/>
       <c r="E36" s="41">
         <f>C36/C34*100</f>
-        <v>83.32919140771449</v>
+        <v>84.310605160710054</v>
       </c>
       <c r="F36" s="51"/>
       <c r="G36" s="50"/>
@@ -2456,19 +2456,19 @@
       <c r="J36" s="50"/>
       <c r="K36" s="51"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="58"/>
       <c r="B37" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="83">
+      <c r="C37" s="87">
         <f>C34-C36</f>
-        <v>38011.332871772116</v>
-      </c>
-      <c r="D37" s="83"/>
+        <v>35357.177353701089</v>
+      </c>
+      <c r="D37" s="87"/>
       <c r="E37" s="41">
         <f>100-E36</f>
-        <v>16.67080859228551</v>
+        <v>15.689394839289946</v>
       </c>
       <c r="F37" s="51"/>
       <c r="G37" s="50"/>
@@ -2477,16 +2477,16 @@
       <c r="J37" s="50"/>
       <c r="K37" s="51"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="58"/>
       <c r="B38" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="83">
+      <c r="C38" s="87">
         <f>C35*0.03</f>
         <v>6000</v>
       </c>
-      <c r="D38" s="83"/>
+      <c r="D38" s="87"/>
       <c r="E38" s="41">
         <v>3</v>
       </c>
@@ -2497,16 +2497,16 @@
       <c r="J38" s="50"/>
       <c r="K38" s="51"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="58"/>
       <c r="B39" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="83">
+      <c r="C39" s="87">
         <f>C35*0.02</f>
         <v>4000</v>
       </c>
-      <c r="D39" s="83"/>
+      <c r="D39" s="87"/>
       <c r="E39" s="41">
         <v>2</v>
       </c>
@@ -2517,7 +2517,7 @@
       <c r="J39" s="50"/>
       <c r="K39" s="51"/>
     </row>
-    <row r="40" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="59"/>
       <c r="B40" s="59"/>
       <c r="C40" s="59"/>
@@ -2530,71 +2530,64 @@
       <c r="J40" s="59"/>
       <c r="K40" s="59"/>
     </row>
-    <row r="41" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="82" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="83" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="84" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="85" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="86" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="87" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="88" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="89" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="90" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="91" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="92" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="93" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="94" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="95" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="96" s="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:11" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="49" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="50" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="51" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="52" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="53" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="54" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="55" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="56" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="57" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="58" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="59" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="60" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="61" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="62" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="63" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="64" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="65" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="66" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="67" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="68" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="69" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="70" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="71" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="72" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="73" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="74" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="75" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="76" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="77" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="78" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="79" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="80" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="81" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="82" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="83" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="84" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="85" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="86" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="87" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="88" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="89" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="90" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="91" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="92" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="93" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="94" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="95" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="96" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="A7:F7"/>
@@ -2603,6 +2596,13 @@
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C37:D37"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>

</xml_diff>